<commit_message>
feat : [조웅현] UserController..?
</commit_message>
<xml_diff>
--- a/산출물/211015_자율프로젝트 교보재 신청_대전_B303.xlsx
+++ b/산출물/211015_자율프로젝트 교보재 신청_대전_B303.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tofan\Desktop\SSAFY_FinalPro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tofan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A74043-57BE-49EF-9FB9-B6E05308B2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49E3886-0A22-4EC5-90A6-CDA92F88F756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="교보재신청" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">교보재신청!$A$1:$R$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">교보재신청!$A$1:$S$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="80">
   <si>
     <t>지역</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -75,6 +75,14 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>도서</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>도서(이북)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -115,10 +123,18 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>기타</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>학번</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>라이선스</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>선/후불</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -147,6 +163,12 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>자바 ORM 표준 JPA 프로그래밍 - 기본편</t>
+  </si>
+  <si>
+    <t>https://www.inflearn.com/course/ORM-JPA-Basic</t>
+  </si>
+  <si>
     <t>스프링 부트와 AWS로 혼자 구현하는 웹 서비스</t>
   </si>
   <si>
@@ -170,6 +192,234 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>스프링</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> MVC 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>편</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>백엔드</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>웹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개발</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>핵심</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기술</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>스프링</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> MVC 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>편</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>백엔드</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>웹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개발</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>활용</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기술</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>프로젝트 수행을 위한 학습 자료</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -203,6 +453,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>스프링 기본기 학습</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>프론트엔드 HTTP 메서드에 대한 이해</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -253,12 +507,19 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>Vue.js + TypeScript 완벽 가이드</t>
+  </si>
+  <si>
     <t>트렐로 개발로 배우는 Vuejs, Vuex, Vue-Router 프론트엔드 실전 기술</t>
   </si>
   <si>
     <t xml:space="preserve">Vuejs 중급 기술 학습 </t>
   </si>
   <si>
+    <t>https://www.inflearn.com/course/vue-ts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>https://www.inflearn.com/course/vuejs#curriculum</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -275,6 +536,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>[OpenCV] 파이썬 딥러닝 영상처리 프로젝트 - 손흥민을 찾아라!</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -287,36 +552,19 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>항목</t>
-  </si>
-  <si>
-    <t>도서</t>
-  </si>
-  <si>
-    <t>도서(이북)</t>
-  </si>
-  <si>
-    <t>강의</t>
-  </si>
-  <si>
-    <t>서버</t>
-  </si>
-  <si>
-    <t>라이선스</t>
-  </si>
-  <si>
-    <t>기타</t>
+    <t>CSS에 날개를 달아주는 Sass (SCSS)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>https://www.inflearn.com/course/css에-날개를-달아주는-sass-scss</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>CSS에 날개를 달아주는 Sass (SCSS)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>CSS 작성시 능률 향상</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>추가</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -328,7 +576,7 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-\$* #,##0.00_ ;_-\$* \-#,##0.00\ ;_-\$* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +620,11 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
@@ -387,6 +640,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
@@ -394,24 +654,7 @@
       <scheme val="major"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
@@ -419,10 +662,22 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -439,7 +694,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -448,16 +703,22 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
+      <left style="medium">
         <color indexed="64"/>
-      </bottom>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -472,38 +733,8 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -520,116 +751,122 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -661,15 +898,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>268941</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>179293</xdr:rowOff>
+      <xdr:colOff>212911</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>104776</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>67234</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>48746</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>11204</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -684,8 +921,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="268941" y="5020234"/>
-          <a:ext cx="13114806" cy="6140824"/>
+          <a:off x="212911" y="4807323"/>
+          <a:ext cx="14448306" cy="5692587"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2096,1030 +2333,1231 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="7.75" style="6" customWidth="1"/>
-    <col min="4" max="4" width="13.875" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.25" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="6" customWidth="1"/>
-    <col min="8" max="8" width="10.625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="58.375" style="13" customWidth="1"/>
-    <col min="10" max="10" width="7.625" customWidth="1"/>
-    <col min="11" max="11" width="13" style="6" customWidth="1"/>
-    <col min="12" max="12" width="17.5" style="6" customWidth="1"/>
-    <col min="13" max="13" width="8" style="5" customWidth="1"/>
-    <col min="14" max="14" width="13" style="4" customWidth="1"/>
-    <col min="15" max="15" width="9.25" customWidth="1"/>
-    <col min="16" max="16" width="13" style="4" customWidth="1"/>
-    <col min="17" max="17" width="21" style="6" customWidth="1"/>
-    <col min="18" max="18" width="15.75" customWidth="1"/>
-    <col min="20" max="20" width="12" customWidth="1"/>
+    <col min="1" max="3" width="7.75" style="13" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.25" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="13" customWidth="1"/>
+    <col min="8" max="8" width="10.625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="31.875" style="27" customWidth="1"/>
+    <col min="10" max="10" width="18.875" customWidth="1"/>
+    <col min="11" max="11" width="13" style="13" customWidth="1"/>
+    <col min="12" max="12" width="55" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.625" style="30" customWidth="1"/>
+    <col min="14" max="14" width="8" style="9" customWidth="1"/>
+    <col min="15" max="15" width="13" style="7" customWidth="1"/>
+    <col min="16" max="16" width="9.25" customWidth="1"/>
+    <col min="17" max="17" width="13" style="7" customWidth="1"/>
+    <col min="18" max="18" width="21" style="13" customWidth="1"/>
+    <col min="19" max="19" width="15.75" customWidth="1"/>
+    <col min="21" max="21" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="G1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="31"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="6">
+        <v>99000</v>
+      </c>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="6">
+        <f>((N2*1300)+O2)*P2</f>
+        <v>99000</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" s="31"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="6">
+        <v>121000</v>
+      </c>
+      <c r="P3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="6">
+        <f t="shared" ref="Q3:Q34" si="0">((N3*1300)+O3)*P3</f>
+        <v>121000</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="13">
+        <v>3</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="N4" s="15"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="6">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="R4" s="3"/>
+      <c r="S4" s="2"/>
+      <c r="U4" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="13">
+        <v>3</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="13"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="6">
+        <v>15400</v>
+      </c>
+      <c r="P5" s="2">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="34"/>
-    </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="14">
-        <v>3</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="M2" s="19"/>
-      <c r="N2" s="20">
-        <v>99000</v>
-      </c>
-      <c r="O2" s="14">
-        <v>1</v>
-      </c>
-      <c r="P2" s="20">
-        <f>((M2*1300)+N2)*O2</f>
-        <v>99000</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14">
-        <v>2</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="14">
-        <v>3</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="M3" s="19"/>
-      <c r="N3" s="20">
-        <v>121000</v>
-      </c>
-      <c r="O3" s="14">
-        <v>1</v>
-      </c>
-      <c r="P3" s="20">
-        <f t="shared" ref="P3:P25" si="0">((M3*1300)+N3)*O3</f>
-        <v>121000</v>
-      </c>
-      <c r="Q3" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="S3" s="28"/>
-      <c r="T3" s="32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14">
-        <v>3</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="17">
-        <v>3</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="17"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="20">
-        <v>15400</v>
-      </c>
-      <c r="O4" s="14">
-        <v>1</v>
-      </c>
-      <c r="P4" s="20">
+      <c r="Q5" s="6">
         <f t="shared" si="0"/>
         <v>15400</v>
       </c>
-      <c r="Q4" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="S4" s="28"/>
-      <c r="T4" s="32" t="s">
-        <v>66</v>
+      <c r="R5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14">
-        <v>4</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="17">
+    <row r="6" spans="1:21" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="13">
         <v>3</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="17" t="s">
+      <c r="D6" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" s="22"/>
-      <c r="N5" s="20">
+      <c r="I6" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" s="31"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="6">
         <v>44000</v>
       </c>
-      <c r="O5" s="14">
+      <c r="P6" s="2">
         <v>1</v>
       </c>
-      <c r="P5" s="20">
+      <c r="Q6" s="6">
         <f t="shared" si="0"/>
         <v>44000</v>
       </c>
-      <c r="Q5" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="R5" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="S5" s="28"/>
-      <c r="T5" s="32" t="s">
-        <v>67</v>
+      <c r="R6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U6" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
-        <v>5</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="17">
+    <row r="7" spans="1:21" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="13">
         <v>3</v>
       </c>
-      <c r="D6" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="17" t="s">
+      <c r="D7" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="20">
+      <c r="I7" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" s="31"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="6">
         <v>69300</v>
       </c>
-      <c r="O6" s="14">
+      <c r="P7" s="2">
         <v>1</v>
       </c>
-      <c r="P6" s="20">
+      <c r="Q7" s="6">
         <f t="shared" si="0"/>
         <v>69300</v>
       </c>
-      <c r="Q6" s="16" t="s">
+      <c r="R7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U7" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="13">
+        <v>3</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="M8" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="N8" s="15"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="3"/>
+      <c r="S8" s="2"/>
+      <c r="U8" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="13">
+        <v>3</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="N9" s="15"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="3"/>
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="13">
+        <v>3</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="R6" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="S6" s="28"/>
-      <c r="T6" s="32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14">
-        <v>6</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="17">
-        <v>3</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" s="17" t="s">
+      <c r="F10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="M7" s="25"/>
-      <c r="N7" s="26">
+      <c r="I10" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="M10" s="29"/>
+      <c r="O10" s="7">
         <v>55000</v>
       </c>
-      <c r="O7" s="14">
+      <c r="P10" s="2">
         <v>1</v>
       </c>
-      <c r="P7" s="20">
+      <c r="Q10" s="6">
         <f t="shared" si="0"/>
         <v>55000</v>
       </c>
-      <c r="Q7" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="R7" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="S7" s="29"/>
-      <c r="T7" s="31" t="s">
-        <v>69</v>
+      <c r="R10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14">
-        <v>7</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="17">
+    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="13">
         <v>3</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="17" t="s">
+      <c r="D11" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="M8" s="25"/>
-      <c r="N8" s="26">
+      <c r="I11" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="13">
+        <v>3</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="M12" s="29"/>
+      <c r="O12" s="7">
         <v>121000</v>
       </c>
-      <c r="O8" s="14">
+      <c r="P12" s="2">
         <v>1</v>
       </c>
-      <c r="P8" s="20">
+      <c r="Q12" s="6">
         <f t="shared" si="0"/>
         <v>121000</v>
       </c>
-      <c r="Q8" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="R8" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="S8" s="29"/>
-      <c r="T8" s="30" t="s">
-        <v>70</v>
+      <c r="R12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14">
+    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="13">
+        <v>3</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="17">
-        <v>3</v>
-      </c>
-      <c r="D9" s="21" t="s">
+      <c r="I13" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="K13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="M9" s="25"/>
-      <c r="N9" s="26">
+      <c r="M13" s="29"/>
+      <c r="O13" s="7">
         <v>88000</v>
       </c>
-      <c r="O9" s="14">
+      <c r="P13" s="2">
         <v>1</v>
       </c>
-      <c r="P9" s="20">
+      <c r="Q13" s="6">
         <f t="shared" si="0"/>
         <v>88000</v>
       </c>
-      <c r="Q9" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="R9" s="14" t="s">
-        <v>52</v>
+      <c r="R13" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14">
-        <v>9</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="17">
+    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="13">
         <v>3</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D14" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="K14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="16" t="s">
+      <c r="M14" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="13">
+        <v>3</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="M15" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="13">
+        <v>3</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="M16" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S16" s="2"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="13">
+        <v>3</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J10" s="23"/>
-      <c r="K10" s="17" t="s">
+      <c r="I17" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="M17" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S17" s="2"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="13">
+        <v>3</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="M18" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S18" s="2"/>
+    </row>
+    <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="L10" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="M10" s="25"/>
-      <c r="N10" s="26">
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="13">
+        <v>3</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="M19" s="29"/>
+      <c r="O19" s="7">
         <v>55000</v>
       </c>
-      <c r="O10" s="14">
+      <c r="P19" s="2">
         <v>1</v>
       </c>
-      <c r="P10" s="20">
+      <c r="Q19" s="6">
         <f t="shared" si="0"/>
         <v>55000</v>
       </c>
-      <c r="Q10" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="R10" s="14" t="s">
-        <v>52</v>
+      <c r="R19" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
-        <v>10</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="17">
+    <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="30">
         <v>3</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="17" t="s">
+      <c r="D20" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" s="23"/>
-      <c r="K11" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="M11" s="25"/>
-      <c r="N11" s="26">
+      <c r="I20" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="34"/>
+      <c r="K20" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="M20" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="O20" s="7">
         <v>55000</v>
       </c>
-      <c r="O11" s="14">
+      <c r="P20" s="2">
         <v>1</v>
       </c>
-      <c r="P11" s="20">
+      <c r="Q20" s="6">
         <f t="shared" si="0"/>
         <v>55000</v>
       </c>
-      <c r="Q11" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="R11" s="14" t="s">
-        <v>52</v>
+      <c r="R20" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
-        <v>11</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="17">
+    <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="30">
         <v>3</v>
       </c>
-      <c r="D12" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="17" t="s">
+      <c r="D21" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="M12" s="25"/>
-      <c r="N12" s="26">
+      <c r="I21" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="J21" s="34"/>
+      <c r="K21" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M21" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="O21" s="7">
         <v>27500</v>
       </c>
-      <c r="O12" s="14">
+      <c r="P21" s="2">
         <v>1</v>
       </c>
-      <c r="P12" s="20">
+      <c r="Q21" s="6">
         <f t="shared" si="0"/>
         <v>27500</v>
       </c>
-      <c r="Q12" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="R12" s="14" t="s">
-        <v>52</v>
+      <c r="R21" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="20">
+    <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q22" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="14"/>
     </row>
-    <row r="14" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="20">
+    <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q23" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="23"/>
     </row>
-    <row r="15" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="20">
+    <row r="24" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q24" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="23"/>
     </row>
-    <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="20">
+    <row r="25" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q25" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="23"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="20">
+    <row r="26" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q26" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="23"/>
     </row>
-    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="20">
+    <row r="27" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q27" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="23"/>
     </row>
-    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="20">
+    <row r="28" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q28" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="23"/>
     </row>
-    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="20">
+    <row r="29" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q29" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="23"/>
     </row>
-    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="20">
+    <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q30" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="23"/>
     </row>
-    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="20">
+    <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q31" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="23"/>
     </row>
-    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="20">
+    <row r="32" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q32" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="23"/>
     </row>
-    <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="20">
+    <row r="33" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q33" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="23"/>
     </row>
-    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="20">
+    <row r="34" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q34" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="23"/>
     </row>
-    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="20">
-        <f>SUM(P2:P25)</f>
+    <row r="35" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q35" s="6">
+        <f>SUM(Q2:Q34)</f>
         <v>750200</v>
       </c>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H13" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H19" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>$U$3:$U$8</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H21" xr:uid="{EED1D581-B926-4517-A5A9-DD94A4DD5EFF}">
       <formula1>$T$3:$T$6</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="L6" r:id="rId1" xr:uid="{4B3E531A-8E62-4283-A378-9932288F364E}"/>
-    <hyperlink ref="L7" r:id="rId2" xr:uid="{105071BE-C126-4AC6-9EAA-23A3B43DD595}"/>
-    <hyperlink ref="L8" r:id="rId3" xr:uid="{4A93316E-E423-4668-A5F3-63F8468FFDC2}"/>
-    <hyperlink ref="L9" r:id="rId4" xr:uid="{6AACCBFA-B237-41F5-B166-6F3208843FC2}"/>
-    <hyperlink ref="L10" r:id="rId5" location="curriculum" xr:uid="{7841571B-F0F4-44D3-B7B1-6EA3FFF8C484}"/>
-    <hyperlink ref="L3" r:id="rId6" xr:uid="{8355F9B0-1726-460D-B4AB-2B8B7447FF7D}"/>
-    <hyperlink ref="L2" r:id="rId7" xr:uid="{A1CA6E73-6054-43B2-90CE-8D84D586E46B}"/>
-    <hyperlink ref="L5" r:id="rId8" xr:uid="{CE8CD914-0D59-4C2E-B0E4-FEFFCC7C20F0}"/>
-    <hyperlink ref="L11" r:id="rId9" xr:uid="{58934E97-FADB-4941-B25D-825A045FFB5A}"/>
-    <hyperlink ref="L12" r:id="rId10" xr:uid="{547CE399-F2AA-4F6D-9E5D-5F7C95193821}"/>
+    <hyperlink ref="L4" r:id="rId1" xr:uid="{A3A5DF87-9899-4EDC-8994-A2A40CA3F3FA}"/>
+    <hyperlink ref="L7" r:id="rId2" xr:uid="{4B3E531A-8E62-4283-A378-9932288F364E}"/>
+    <hyperlink ref="L8" r:id="rId3" xr:uid="{7F78BE19-466D-4679-B918-85FD92200651}"/>
+    <hyperlink ref="L9" r:id="rId4" xr:uid="{AA601D8F-D2A2-4710-ADEC-53412D2B6982}"/>
+    <hyperlink ref="L10" r:id="rId5" xr:uid="{105071BE-C126-4AC6-9EAA-23A3B43DD595}"/>
+    <hyperlink ref="L11" r:id="rId6" xr:uid="{4EAAF592-A4FD-4374-A278-A9B779EEFC96}"/>
+    <hyperlink ref="L12" r:id="rId7" xr:uid="{4A93316E-E423-4668-A5F3-63F8468FFDC2}"/>
+    <hyperlink ref="L13" r:id="rId8" xr:uid="{6AACCBFA-B237-41F5-B166-6F3208843FC2}"/>
+    <hyperlink ref="L14" r:id="rId9" xr:uid="{FAAF56F2-4CBC-48E1-8516-047206A477F7}"/>
+    <hyperlink ref="L15" r:id="rId10" xr:uid="{D022D1E4-2CD8-48F9-9140-21B350655268}"/>
+    <hyperlink ref="L16" r:id="rId11" xr:uid="{95606043-7DD3-452B-97E8-90ADE3503506}"/>
+    <hyperlink ref="L17" r:id="rId12" xr:uid="{DA5437E3-A524-4C15-9D44-A2A279203101}"/>
+    <hyperlink ref="L18" r:id="rId13" xr:uid="{3C2D3114-1BAE-4956-ABD6-AD29E7863431}"/>
+    <hyperlink ref="L19" r:id="rId14" location="curriculum" xr:uid="{7841571B-F0F4-44D3-B7B1-6EA3FFF8C484}"/>
+    <hyperlink ref="L3" r:id="rId15" xr:uid="{8355F9B0-1726-460D-B4AB-2B8B7447FF7D}"/>
+    <hyperlink ref="L2" r:id="rId16" xr:uid="{A1CA6E73-6054-43B2-90CE-8D84D586E46B}"/>
+    <hyperlink ref="L6" r:id="rId17" xr:uid="{CE8CD914-0D59-4C2E-B0E4-FEFFCC7C20F0}"/>
+    <hyperlink ref="L20" r:id="rId18" xr:uid="{5BCD9CD5-17E0-4914-A688-9C6D932A5955}"/>
+    <hyperlink ref="L21" r:id="rId19" xr:uid="{190967AF-8950-4DBB-B4D5-88196DBCEFFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
-  <drawing r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <drawing r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>